<commit_message>
script do jogo iniciado
</commit_message>
<xml_diff>
--- a/SI401_ContribuicaoIndividualTrabalho.xlsx
+++ b/SI401_ContribuicaoIndividualTrabalho.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilherme\OneDrive - Universidade Estadual de Campinas\Unicamp\FT\Disciplinas\2020\2s2020\SI401\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Capitetris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{9422C08C-0E34-4068-B510-B8B3993F4587}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{1A40AD54-D74A-4F8A-BCAC-D2D798219082}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BBC551-E9FA-45D5-87BE-443DDF9211B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{8AD44023-9501-48E1-8BFC-2E44CC22AE8A}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{8AD44023-9501-48E1-8BFC-2E44CC22AE8A}"/>
   </bookViews>
   <sheets>
     <sheet name="Contribuição Individual" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,21 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Relatório de Contribuição Individual</t>
   </si>
@@ -96,19 +105,37 @@
     <t xml:space="preserve">      B = mínimo (10,0; (Nota do Grupo no Trabalho + 1,0)).</t>
   </si>
   <si>
-    <t>Donald Duck</t>
-  </si>
-  <si>
-    <t>Minnie Mouse</t>
-  </si>
-  <si>
-    <t>Contribuiu com a metade mais importante do trabalho.</t>
-  </si>
-  <si>
-    <t>Contribuiu com a metade menos importante do trabalho.</t>
-  </si>
-  <si>
     <t>Nota do Grupo no Trabalho (será atribuída pelo professor):</t>
+  </si>
+  <si>
+    <t>Grupo_09</t>
+  </si>
+  <si>
+    <t>Rolling Tetris (Capiteris)</t>
+  </si>
+  <si>
+    <t>Arthur Felipe</t>
+  </si>
+  <si>
+    <t>Eric Satoshi Suzuki Kishimoto</t>
+  </si>
+  <si>
+    <t>Verônica Cintra de Oliveira</t>
+  </si>
+  <si>
+    <t>Vitor Roberto Kogawa de Moraes</t>
+  </si>
+  <si>
+    <t>Contribuiu para criar design da interface, codificar as páginas HTML e editou o vídeo</t>
+  </si>
+  <si>
+    <t>Contribuiu para criar design da interface, codificar as páginas HTML e administrar o projeto</t>
+  </si>
+  <si>
+    <t>Contribuiu para criar design da interface, codificar as páginas HTML e codificou a responsabilidade do site</t>
+  </si>
+  <si>
+    <t>Contribuiu para criar design da interface, codificar as páginas HTML e deu a ideia do design do site</t>
   </si>
 </sst>
 </file>
@@ -401,10 +428,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -441,6 +464,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -812,21 +839,21 @@
   </sheetPr>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="90" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.5703125" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.5546875" customWidth="1"/>
+    <col min="6" max="6" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -836,7 +863,7 @@
       <c r="E1" s="43"/>
       <c r="F1" s="44"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="45" t="s">
         <v>7</v>
       </c>
@@ -846,27 +873,31 @@
       <c r="E2" s="46"/>
       <c r="F2" s="47"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="49" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="49"/>
-      <c r="C3" s="48"/>
+      <c r="C3" s="48" t="s">
+        <v>24</v>
+      </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
       <c r="F3" s="48"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="48"/>
+      <c r="C4" s="48" t="s">
+        <v>25</v>
+      </c>
       <c r="D4" s="48"/>
       <c r="E4" s="48"/>
       <c r="F4" s="48"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -874,19 +905,17 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="40" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
       <c r="E6" s="41"/>
-      <c r="F6" s="32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="31"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -894,7 +923,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -912,101 +941,117 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>1</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="20">
-        <v>123456</v>
-      </c>
-      <c r="D9" s="24">
-        <v>0.501</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="31">
+        <v>26</v>
+      </c>
+      <c r="C9" s="21">
+        <v>231661</v>
+      </c>
+      <c r="D9" s="23">
+        <v>0.252</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="30">
         <f>IF(D9="","",IF($A$18="",ROUND(MIN(MIN(10,$F$6+1),COUNTA($D$9:$D$13)*$F$6*D9),1),"Erro"))</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>2</v>
       </c>
-      <c r="B10" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="22">
-        <v>999123</v>
-      </c>
-      <c r="D10" s="25">
-        <v>0.499</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F10" s="31">
+      <c r="B10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="21">
+        <v>233974</v>
+      </c>
+      <c r="D10" s="24">
+        <v>0.251</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="30">
         <f t="shared" ref="F10:F13" si="0">IF(D10="","",IF($A$18="",ROUND(MIN(MIN(10,$F$6+1),COUNTA($D$9:$D$13)*$F$6*D10),1),"Erro"))</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>3</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="31" t="str">
+      <c r="B11" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="33">
+        <v>244963</v>
+      </c>
+      <c r="D11" s="24">
+        <v>0.249</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="21">
+        <v>245582</v>
+      </c>
+      <c r="D12" s="24">
+        <v>0.248</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="10">
+        <v>5</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="30" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
-        <v>4</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
-        <v>5</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="31" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="40" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="41"/>
       <c r="C14" s="41"/>
-      <c r="D14" s="26">
+      <c r="D14" s="25">
         <f>1 - SUM(D9:D13)</f>
         <v>0</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="13"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1014,7 +1059,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="34" t="s">
         <v>9</v>
       </c>
@@ -1024,10 +1069,10 @@
       <c r="E16" s="36"/>
       <c r="F16" s="6">
         <f ca="1">NOW()</f>
-        <v>44082.731292129632</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44126.678782754629</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
@@ -1035,7 +1080,7 @@
       <c r="E17" s="14"/>
       <c r="F17" s="13"/>
     </row>
-    <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="str">
         <f>IF(SUM(D9:D13)=1,"","ATENÇÃO: A soma dos valores da coluna 'Contribuição (%)' deve ser 100%.")</f>
         <v/>
@@ -1046,7 +1091,7 @@
       <c r="E18" s="38"/>
       <c r="F18" s="39"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1054,8 +1099,8 @@
       <c r="E19" s="12"/>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="33" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="12"/>
@@ -1064,9 +1109,9 @@
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="11"/>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="12"/>
@@ -1074,9 +1119,9 @@
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="12"/>
@@ -1084,9 +1129,9 @@
       <c r="E22" s="12"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C23" s="12"/>
@@ -1094,9 +1139,9 @@
       <c r="E23" s="12"/>
       <c r="F23" s="13"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="12"/>
@@ -1104,9 +1149,9 @@
       <c r="E24" s="12"/>
       <c r="F24" s="13"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="12"/>
@@ -1114,9 +1159,9 @@
       <c r="E25" s="12"/>
       <c r="F25" s="13"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="12"/>
@@ -1124,9 +1169,9 @@
       <c r="E26" s="12"/>
       <c r="F26" s="13"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="12"/>
@@ -1134,9 +1179,9 @@
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="12"/>
@@ -1144,9 +1189,9 @@
       <c r="E28" s="12"/>
       <c r="F28" s="13"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="11"/>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>20</v>
       </c>
       <c r="C29" s="12"/>
@@ -1154,9 +1199,9 @@
       <c r="E29" s="12"/>
       <c r="F29" s="13"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="11"/>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>21</v>
       </c>
       <c r="C30" s="12"/>
@@ -1164,9 +1209,9 @@
       <c r="E30" s="12"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="11"/>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>22</v>
       </c>
       <c r="C31" s="12"/>
@@ -1174,73 +1219,73 @@
       <c r="E31" s="12"/>
       <c r="F31" s="13"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="11"/>
-      <c r="B32" s="29"/>
+      <c r="B32" s="28"/>
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
       <c r="F32" s="13"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="11"/>
-      <c r="B33" s="29"/>
+      <c r="B33" s="28"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
       <c r="F33" s="13"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="11"/>
-      <c r="B34" s="29"/>
+      <c r="B34" s="28"/>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
       <c r="F34" s="13"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="11"/>
-      <c r="B35" s="29"/>
+      <c r="B35" s="28"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="13"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="11"/>
-      <c r="B36" s="29"/>
+      <c r="B36" s="28"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="11"/>
-      <c r="B37" s="29"/>
+      <c r="B37" s="28"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
       <c r="F37" s="13"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="11"/>
-      <c r="B38" s="29"/>
+      <c r="B38" s="28"/>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="13"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="11"/>
-      <c r="B39" s="29"/>
+      <c r="B39" s="28"/>
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
       <c r="F39" s="13"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="15"/>
-      <c r="B40" s="30"/>
+      <c r="B40" s="29"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
       <c r="E40" s="16"/>
@@ -1276,6 +1321,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010027B1B795F3ACD74191B7284862A64588" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="9ae5dfd6e757cdf140f76020e29a6e0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="de106b6a-02b6-4774-b219-e71fbb5cc1ce" xmlns:ns4="5feea0e9-8f6d-471c-b84e-b049251fc55f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d30e59c414edc37baddb95c666cd0950" ns3:_="" ns4:_="">
     <xsd:import namespace="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
@@ -1498,7 +1549,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1507,13 +1558,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0537F2A3-82D8-4D11-AF44-B60EFF661ED7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="5feea0e9-8f6d-471c-b84e-b049251fc55f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{674BDE44-CA73-45BE-9BAA-FE3EA527B3F3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1532,27 +1594,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDDB3412-F176-463C-9CD3-ADF26C83D016}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0537F2A3-82D8-4D11-AF44-B60EFF661ED7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="5feea0e9-8f6d-471c-b84e-b049251fc55f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="de106b6a-02b6-4774-b219-e71fbb5cc1ce"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>